<commit_message>
Ready for Part D insertion
</commit_message>
<xml_diff>
--- a/HT36C/A4_HT36C_B_1.xlsx
+++ b/HT36C/A4_HT36C_B_1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smtgn\Desktop\S19\Thermal Fluids\GitHub\24321-A4\HT36C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/PKBACK# 001/GitHub/24321-A4/HT36C/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EE4E90-61D5-4358-9E63-53E4ACAF344B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71F6900-6A27-F449-B721-4F0045215A08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{87300929-A993-419C-A33A-943911ED9D89}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24720" windowHeight="13840" xr2:uid="{87300929-A993-419C-A33A-943911ED9D89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -151,36 +151,6 @@
   </si>
   <si>
     <t>4</t>
-  </si>
-  <si>
-    <t>T6</t>
-  </si>
-  <si>
-    <t>T7</t>
-  </si>
-  <si>
-    <t>T8</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T9</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T10</t>
   </si>
 </sst>
 </file>
@@ -204,6 +174,7 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -597,12 +568,12 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" ht="73.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" ht="84" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,43 +644,45 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="4">
-        <v>15.845703125</v>
+        <v>43.738037109375</v>
       </c>
       <c r="D2" s="4">
-        <v>15.91064453125</v>
+        <v>44.971923828125</v>
       </c>
       <c r="E2" s="4">
-        <v>15.91064453125</v>
+        <v>46.595458984375</v>
       </c>
       <c r="F2" s="4">
-        <v>16.137939453125</v>
+        <v>48.998291015625</v>
       </c>
       <c r="G2" s="4">
-        <v>16.17041015625</v>
+        <v>53.479248046875</v>
       </c>
       <c r="H2" s="4">
         <v>14.189697265625</v>
       </c>
       <c r="I2" s="4">
-        <v>14.48193359375</v>
+        <v>23.7685546875</v>
       </c>
       <c r="J2" s="4">
-        <v>14.4169921875</v>
+        <v>28.801513671875</v>
       </c>
       <c r="K2" s="4">
-        <v>15.00146484375</v>
+        <v>32.503173828125</v>
       </c>
       <c r="L2" s="4">
-        <v>15.13134765625</v>
+        <v>35.52294921875</v>
       </c>
       <c r="M2" s="5">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N2" s="4">
         <v>1.98974609375</v>
@@ -718,308 +691,341 @@
         <v>44</v>
       </c>
       <c r="P2" s="6">
-        <v>0.98876953125</v>
+        <v>1.01318359375</v>
       </c>
       <c r="Q2" s="7">
         <v>0</v>
       </c>
       <c r="R2" s="5" t="str">
-        <f t="shared" ref="R2:R17" si="0">IF(ISNUMBER(E2),IF(ROW(A2)=2,"Cocurrent",""),"")</f>
+        <f>IF(ISNUMBER(E2),IF(ROW(A2)=2,"Cocurrent",""),"")</f>
         <v>Cocurrent</v>
       </c>
-      <c r="S2" s="8" t="s">
-        <v>29</v>
+      <c r="S2" s="8" t="str">
+        <f t="shared" ref="S2:S6" si="0">IF(ISNUMBER(E$2),IF(ROW(A2)=6,IF(B$2="4","T1",""),IF(ROW(A2)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A2)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A2)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A2)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <v>T5</v>
       </c>
       <c r="T2" s="9">
-        <v>16.17041015625</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>24</v>
+        <f t="shared" ref="T2:T6" si="1">IF(S2="T1",C$2,IF(S2="T2",D$2,IF(S2="T3",E$2,IF(S2="T4",F$2,IF(S2="T5",G$2,"")))))</f>
+        <v>53.479248046875</v>
+      </c>
+      <c r="U2" s="5" t="str">
+        <f t="shared" ref="U2:U6" si="2">IF(ISNUMBER(E$2),IF(ROW(A2)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A2)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A2)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A2)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A2)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <v>T6</v>
       </c>
       <c r="V2" s="9">
+        <f t="shared" ref="V2:V6" si="3">IF(U2="T6",H$2,IF(U2="T7",I$2,IF(U2="T8",J$2,IF(U2="T9",K$2,IF(U2="T10",L$2,"")))))</f>
         <v>14.189697265625</v>
       </c>
       <c r="W2" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0</v>
-      </c>
-      <c r="O3" s="3">
-        <v>0</v>
-      </c>
-      <c r="P3" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>28</v>
+        <f t="shared" ref="W2:W6" si="4">IF(ISNUMBER(E$2),IF(ROW($A2)=2,0,IF(ROW($A2)=3,670,IF(ROW($A2)=4,IF((B$2)="1","",1340),IF(ROW($A2)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A2)=6,IF(B$2="4",2680,""),""))))),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0</v>
+      </c>
+      <c r="S3" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T4</v>
       </c>
       <c r="T3" s="9">
-        <v>16.137939453125</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>48.998291015625</v>
+      </c>
+      <c r="U3" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>T7</v>
       </c>
       <c r="V3" s="9">
-        <v>14.48193359375</v>
+        <f t="shared" si="3"/>
+        <v>23.7685546875</v>
       </c>
       <c r="W3" s="10">
+        <f t="shared" si="4"/>
         <v>670</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3">
-        <v>0</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>27</v>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T3</v>
       </c>
       <c r="T4" s="9">
-        <v>15.91064453125</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>46.595458984375</v>
+      </c>
+      <c r="U4" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>T8</v>
       </c>
       <c r="V4" s="9">
-        <v>14.4169921875</v>
+        <f t="shared" si="3"/>
+        <v>28.801513671875</v>
       </c>
       <c r="W4" s="10">
+        <f t="shared" si="4"/>
         <v>1340</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>0</v>
-      </c>
-      <c r="R5" s="3">
-        <v>0</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>30</v>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T2</v>
       </c>
       <c r="T5" s="9">
-        <v>15.91064453125</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>44.971923828125</v>
+      </c>
+      <c r="U5" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>T9</v>
       </c>
       <c r="V5" s="9">
-        <v>15.00146484375</v>
+        <f t="shared" si="3"/>
+        <v>32.503173828125</v>
       </c>
       <c r="W5" s="10">
+        <f t="shared" si="4"/>
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>32</v>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0</v>
+      </c>
+      <c r="S6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T1</v>
       </c>
       <c r="T6" s="9">
-        <v>15.845703125</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>43.738037109375</v>
+      </c>
+      <c r="U6" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>T10</v>
       </c>
       <c r="V6" s="9">
-        <v>15.13134765625</v>
+        <f t="shared" si="3"/>
+        <v>35.52294921875</v>
       </c>
       <c r="W6" s="10">
+        <f t="shared" si="4"/>
         <v>2680</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1038,31 +1044,31 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="R7:R17" si="5">IF(ISNUMBER(E7),IF(ROW(A7)=2,"Cocurrent",""),"")</f>
         <v/>
       </c>
       <c r="S7" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A7)=6,IF(B$2="4","T1",""),IF(ROW(A7)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A7)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A7)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A7)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" ref="S7:S17" si="6">IF(ISNUMBER(E$2),IF(ROW(A7)=6,IF(B$2="4","T1",""),IF(ROW(A7)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A7)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A7)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A7)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
         <v/>
       </c>
       <c r="T7" s="9" t="str">
-        <f>IF(S7="T1",C$2,IF(S7="T2",D$2,IF(S7="T3",E$2,IF(S7="T4",F$2,IF(S7="T5",G$2,"")))))</f>
+        <f t="shared" ref="T7:T17" si="7">IF(S7="T1",C$2,IF(S7="T2",D$2,IF(S7="T3",E$2,IF(S7="T4",F$2,IF(S7="T5",G$2,"")))))</f>
         <v/>
       </c>
       <c r="U7" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A7)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A7)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A7)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A7)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A7)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" ref="U7:U17" si="8">IF(ISNUMBER(E$2),IF(ROW(A7)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A7)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A7)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A7)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A7)=6,IF(B$2="4","T10",""),""))))),"")</f>
         <v/>
       </c>
       <c r="V7" s="9" t="str">
-        <f>IF(U7="T6",H$2,IF(U7="T7",I$2,IF(U7="T8",J$2,IF(U7="T9",K$2,IF(U7="T10",L$2,"")))))</f>
+        <f t="shared" ref="V7:V17" si="9">IF(U7="T6",H$2,IF(U7="T7",I$2,IF(U7="T8",J$2,IF(U7="T9",K$2,IF(U7="T10",L$2,"")))))</f>
         <v/>
       </c>
       <c r="W7" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A7)=2,0,IF(ROW($A7)=3,670,IF(ROW($A7)=4,IF((B$2)="1","",1340),IF(ROW($A7)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A7)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="W7:W17" si="10">IF(ISNUMBER(E$2),IF(ROW($A7)=2,0,IF(ROW($A7)=3,670,IF(ROW($A7)=4,IF((B$2)="1","",1340),IF(ROW($A7)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A7)=6,IF(B$2="4",2680,""),""))))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -1081,31 +1087,31 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S8" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A8)=6,IF(B$2="4","T1",""),IF(ROW(A8)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A8)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A8)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A8)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T8" s="9" t="str">
-        <f>IF(S8="T1",C$2,IF(S8="T2",D$2,IF(S8="T3",E$2,IF(S8="T4",F$2,IF(S8="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U8" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A8)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A8)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A8)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A8)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A8)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V8" s="9" t="str">
-        <f>IF(U8="T6",H$2,IF(U8="T7",I$2,IF(U8="T8",J$2,IF(U8="T9",K$2,IF(U8="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W8" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A8)=2,0,IF(ROW($A8)=3,670,IF(ROW($A8)=4,IF((B$2)="1","",1340),IF(ROW($A8)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A8)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1124,31 +1130,31 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S9" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A9)=6,IF(B$2="4","T1",""),IF(ROW(A9)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A9)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A9)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A9)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T9" s="9" t="str">
-        <f>IF(S9="T1",C$2,IF(S9="T2",D$2,IF(S9="T3",E$2,IF(S9="T4",F$2,IF(S9="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U9" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A9)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A9)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A9)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A9)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A9)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V9" s="9" t="str">
-        <f>IF(U9="T6",H$2,IF(U9="T7",I$2,IF(U9="T8",J$2,IF(U9="T9",K$2,IF(U9="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W9" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A9)=2,0,IF(ROW($A9)=3,670,IF(ROW($A9)=4,IF((B$2)="1","",1340),IF(ROW($A9)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A9)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1167,31 +1173,31 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S10" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A10)=6,IF(B$2="4","T1",""),IF(ROW(A10)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A10)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A10)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A10)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T10" s="9" t="str">
-        <f>IF(S10="T1",C$2,IF(S10="T2",D$2,IF(S10="T3",E$2,IF(S10="T4",F$2,IF(S10="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U10" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A10)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A10)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A10)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A10)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A10)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V10" s="9" t="str">
-        <f>IF(U10="T6",H$2,IF(U10="T7",I$2,IF(U10="T8",J$2,IF(U10="T9",K$2,IF(U10="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W10" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A10)=2,0,IF(ROW($A10)=3,670,IF(ROW($A10)=4,IF((B$2)="1","",1340),IF(ROW($A10)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A10)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1210,31 +1216,31 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S11" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A11)=6,IF(B$2="4","T1",""),IF(ROW(A11)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A11)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A11)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A11)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T11" s="9" t="str">
-        <f>IF(S11="T1",C$2,IF(S11="T2",D$2,IF(S11="T3",E$2,IF(S11="T4",F$2,IF(S11="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U11" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A11)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A11)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A11)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A11)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A11)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V11" s="9" t="str">
-        <f>IF(U11="T6",H$2,IF(U11="T7",I$2,IF(U11="T8",J$2,IF(U11="T9",K$2,IF(U11="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W11" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A11)=2,0,IF(ROW($A11)=3,670,IF(ROW($A11)=4,IF((B$2)="1","",1340),IF(ROW($A11)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A11)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1253,31 +1259,31 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S12" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A12)=6,IF(B$2="4","T1",""),IF(ROW(A12)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A12)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A12)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A12)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T12" s="9" t="str">
-        <f>IF(S12="T1",C$2,IF(S12="T2",D$2,IF(S12="T3",E$2,IF(S12="T4",F$2,IF(S12="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U12" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A12)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A12)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A12)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A12)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A12)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V12" s="9" t="str">
-        <f>IF(U12="T6",H$2,IF(U12="T7",I$2,IF(U12="T8",J$2,IF(U12="T9",K$2,IF(U12="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W12" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A12)=2,0,IF(ROW($A12)=3,670,IF(ROW($A12)=4,IF((B$2)="1","",1340),IF(ROW($A12)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A12)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1296,31 +1302,31 @@
       <c r="P13" s="6"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S13" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A13)=6,IF(B$2="4","T1",""),IF(ROW(A13)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A13)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A13)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A13)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T13" s="9" t="str">
-        <f>IF(S13="T1",C$2,IF(S13="T2",D$2,IF(S13="T3",E$2,IF(S13="T4",F$2,IF(S13="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U13" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A13)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A13)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A13)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A13)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A13)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V13" s="9" t="str">
-        <f>IF(U13="T6",H$2,IF(U13="T7",I$2,IF(U13="T8",J$2,IF(U13="T9",K$2,IF(U13="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W13" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A13)=2,0,IF(ROW($A13)=3,670,IF(ROW($A13)=4,IF((B$2)="1","",1340),IF(ROW($A13)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A13)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1339,31 +1345,31 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S14" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A14)=6,IF(B$2="4","T1",""),IF(ROW(A14)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A14)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A14)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A14)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T14" s="9" t="str">
-        <f>IF(S14="T1",C$2,IF(S14="T2",D$2,IF(S14="T3",E$2,IF(S14="T4",F$2,IF(S14="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U14" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A14)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A14)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A14)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A14)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A14)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V14" s="9" t="str">
-        <f>IF(U14="T6",H$2,IF(U14="T7",I$2,IF(U14="T8",J$2,IF(U14="T9",K$2,IF(U14="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W14" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A14)=2,0,IF(ROW($A14)=3,670,IF(ROW($A14)=4,IF((B$2)="1","",1340),IF(ROW($A14)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A14)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1382,31 +1388,31 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S15" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A15)=6,IF(B$2="4","T1",""),IF(ROW(A15)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A15)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A15)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A15)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T15" s="9" t="str">
-        <f>IF(S15="T1",C$2,IF(S15="T2",D$2,IF(S15="T3",E$2,IF(S15="T4",F$2,IF(S15="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U15" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A15)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A15)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A15)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A15)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A15)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V15" s="9" t="str">
-        <f>IF(U15="T6",H$2,IF(U15="T7",I$2,IF(U15="T8",J$2,IF(U15="T9",K$2,IF(U15="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W15" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A15)=2,0,IF(ROW($A15)=3,670,IF(ROW($A15)=4,IF((B$2)="1","",1340),IF(ROW($A15)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A15)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1425,31 +1431,31 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S16" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A16)=6,IF(B$2="4","T1",""),IF(ROW(A16)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A16)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A16)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A16)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T16" s="9" t="str">
-        <f>IF(S16="T1",C$2,IF(S16="T2",D$2,IF(S16="T3",E$2,IF(S16="T4",F$2,IF(S16="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U16" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A16)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A16)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A16)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A16)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A16)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V16" s="9" t="str">
-        <f>IF(U16="T6",H$2,IF(U16="T7",I$2,IF(U16="T8",J$2,IF(U16="T9",K$2,IF(U16="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W16" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A16)=2,0,IF(ROW($A16)=3,670,IF(ROW($A16)=4,IF((B$2)="1","",1340),IF(ROW($A16)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A16)=6,IF(B$2="4",2680,""),""))))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1468,27 +1474,27 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S17" s="8" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A17)=6,IF(B$2="4","T1",""),IF(ROW(A17)=5,IF(B$2="4","T2",IF(B$2="3","T1","")),IF(ROW(A17)=4,IF(B$2="4","T3",IF(B$2="3","T2",IF(B$2="2","T1",""))),IF(ROW(A17)=3,IF(B$2="4","T4",IF(B$2="3","T3",IF(B$2="2","T2","T1"))),IF(ROW(A17)=2,IF(B$2="4","T5",IF(B$2="3","T4",IF(B$2="2","T3","T2"))),""))))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T17" s="9" t="str">
-        <f>IF(S17="T1",C$2,IF(S17="T2",D$2,IF(S17="T3",E$2,IF(S17="T4",F$2,IF(S17="T5",G$2,"")))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U17" s="5" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW(A17)=2,IF(B$2="2","T8",IF(B$2="3","T7",IF(B$2="4","T6","T9"))),IF(ROW(A17)=3,IF(B$2="2","T9",IF(B$2="3","T8",IF(B$2="4","T7","T10"))),IF(ROW(A17)=4,IF(B$2="3","T9",IF(B$2="4","T8",IF(B$2="2","T10",""))),IF(ROW(A17)=5,IF(B$2="4","T9",IF(B$2="3","T10","")),IF(ROW(A17)=6,IF(B$2="4","T10",""),""))))),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V17" s="9" t="str">
-        <f>IF(U17="T6",H$2,IF(U17="T7",I$2,IF(U17="T8",J$2,IF(U17="T9",K$2,IF(U17="T10",L$2,"")))))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W17" s="10" t="str">
-        <f>IF(ISNUMBER(E$2),IF(ROW($A17)=2,0,IF(ROW($A17)=3,670,IF(ROW($A17)=4,IF((B$2)="1","",1340),IF(ROW($A17)=5,IF(B$2="1","",IF(B$2="2","",2010)),IF(ROW($A17)=6,IF(B$2="4",2680,""),""))))),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>

</xml_diff>